<commit_message>
Ajout de données d'exemple (multi-attributaire), nouveaux champs #5
</commit_message>
<xml_diff>
--- a/exemples/exemple-valide.xlsx
+++ b/exemples/exemple-valide.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -79,10 +79,19 @@
     <t xml:space="preserve">titulaire.denominationSociale</t>
   </si>
   <si>
+    <t xml:space="preserve">objetModification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donneesActuelles</t>
+  </si>
+  <si>
     <t xml:space="preserve">201900056462300</t>
   </si>
   <si>
-    <t xml:space="preserve">23350001600040201900056462300 </t>
+    <t xml:space="preserve">23350001600040201900056462300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23350001600040</t>
   </si>
   <si>
     <t xml:space="preserve">Conseil régional de Bretagne</t>
@@ -91,7 +100,7 @@
     <t xml:space="preserve">Marché</t>
   </si>
   <si>
-    <t xml:space="preserve">Impression d'affiches pour l'évènement Urban Trail</t>
+    <t xml:space="preserve">Impression d'affiches, de flyer et de dépliants pour l'évènement Urban Trail</t>
   </si>
   <si>
     <t xml:space="preserve">79311000</t>
@@ -100,6 +109,9 @@
     <t xml:space="preserve">Procédure adaptée</t>
   </si>
   <si>
+    <t xml:space="preserve">35238</t>
+  </si>
+  <si>
     <t xml:space="preserve">Code commune</t>
   </si>
   <si>
@@ -118,10 +130,40 @@
     <t xml:space="preserve">Ferme</t>
   </si>
   <si>
+    <t xml:space="preserve">81223113200034</t>
+  </si>
+  <si>
     <t xml:space="preserve">SIRET</t>
   </si>
   <si>
     <t xml:space="preserve">Colin Maudry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82379887100013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datactivist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201900056462301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23350001600040201900056462301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-05-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-06-08  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Augmentation de la durée du marché à 6 mois.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impression d'affiches, de flyer et de dépliants pour l'évènement Urban Traill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-06-08</t>
   </si>
 </sst>
 </file>
@@ -222,20 +264,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R21" activeCellId="0" sqref="R21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
@@ -249,6 +291,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="19.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="39.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,64 +353,265 @@
       <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>23350001600040</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>35238</v>
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="1" t="n">
-        <v>81223113200034</v>
-      </c>
-      <c r="R2" s="0" t="s">
+      <c r="L3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour des exemples ODS et XLSX, suppression de l'exemple XLS
</commit_message>
<xml_diff>
--- a/exemples/exemple-valide.xlsx
+++ b/exemples/exemple-valide.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">donneesActuelles</t>
   </si>
   <si>
+    <t xml:space="preserve">anomalies</t>
+  </si>
+  <si>
     <t xml:space="preserve">201900056462300</t>
   </si>
   <si>
@@ -154,16 +157,10 @@
     <t xml:space="preserve">2019-05-30</t>
   </si>
   <si>
-    <t xml:space="preserve">2019-06-08  </t>
+    <t xml:space="preserve">2019-06-08</t>
   </si>
   <si>
     <t xml:space="preserve">Augmentation de la durée du marché à 6 mois.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impression d'affiches, de flyer et de dépliants pour l'évènement Urban Traill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019-06-08</t>
   </si>
 </sst>
 </file>
@@ -264,7 +261,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -277,7 +274,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="61.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.86"/>
@@ -293,6 +290,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,64 +357,67 @@
       <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U2" s="0" t="n">
         <v>0</v>
@@ -424,61 +425,61 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>0</v>
@@ -486,64 +487,64 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>6</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>1</v>
@@ -551,64 +552,64 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>6</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="U5" s="0" t="n">
         <v>1</v>

</xml_diff>